<commit_message>
Add trustLevel in flow
</commit_message>
<xml_diff>
--- a/exemples/output/A1_Diagram1.xlsx
+++ b/exemples/output/A1_Diagram1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="19">
   <si>
     <t>ID</t>
   </si>
@@ -32,16 +32,22 @@
     <t>Microservice</t>
   </si>
   <si>
+    <t>PROM_PROC</t>
+  </si>
+  <si>
+    <t>Publish message</t>
+  </si>
+  <si>
+    <t>Administration</t>
+  </si>
+  <si>
+    <t>MyProcess</t>
+  </si>
+  <si>
     <t>PROC_RABBIT</t>
   </si>
   <si>
-    <t>Publish message</t>
-  </si>
-  <si>
-    <t>Unknown</t>
-  </si>
-  <si>
-    <t>MyProcess</t>
+    <t>Operational</t>
   </si>
   <si>
     <t>PROC_KAFKA</t>
@@ -56,19 +62,16 @@
     <t>Level of Authorization</t>
   </si>
   <si>
+    <t>Enablers2</t>
+  </si>
+  <si>
+    <t>Enabler services provided</t>
+  </si>
+  <si>
+    <t>Application data</t>
+  </si>
+  <si>
     <t>Enablers</t>
-  </si>
-  <si>
-    <t>Enabler services provided</t>
-  </si>
-  <si>
-    <t>Operational</t>
-  </si>
-  <si>
-    <t>Application data</t>
-  </si>
-  <si>
-    <t>Enablers2</t>
   </si>
 </sst>
 </file>
@@ -116,8 +119,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E4" totalsRowShown="0">
-  <autoFilter ref="A1:E4"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E5" totalsRowShown="0">
+  <autoFilter ref="A1:E5"/>
   <tableColumns count="5">
     <tableColumn id="1" name="ID"/>
     <tableColumn id="2" name="Name"/>
@@ -427,7 +430,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -435,7 +438,7 @@
   <cols>
     <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -484,7 +487,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>8</v>
@@ -492,18 +495,35 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="E4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" t="s">
         <v>8</v>
       </c>
     </row>
@@ -537,38 +557,38 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="D2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add direction and asset name into entry point and add vectors list
</commit_message>
<xml_diff>
--- a/exemples/output/A1_Diagram1.xlsx
+++ b/exemples/output/A1_Diagram1.xlsx
@@ -12,13 +12,14 @@
     <sheet name="Trust Boundaries" sheetId="3" r:id="rId3"/>
     <sheet name="Asset worksheet" sheetId="4" r:id="rId4"/>
     <sheet name="Threats" sheetId="5" r:id="rId5"/>
+    <sheet name="Vectors" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="51">
   <si>
     <t>Name</t>
   </si>
@@ -77,12 +78,21 @@
     <t>ID</t>
   </si>
   <si>
+    <t>Direction</t>
+  </si>
+  <si>
+    <t>Asset Name</t>
+  </si>
+  <si>
     <t>Microservice</t>
   </si>
   <si>
     <t>PROM_PROC</t>
   </si>
   <si>
+    <t>Entry</t>
+  </si>
+  <si>
     <t>Publish message</t>
   </si>
   <si>
@@ -92,6 +102,12 @@
     <t>PROC_RABBIT</t>
   </si>
   <si>
+    <t>Exit</t>
+  </si>
+  <si>
+    <t>OpenApi</t>
+  </si>
+  <si>
     <t>PROC_KAFKA</t>
   </si>
   <si>
@@ -104,19 +120,16 @@
     <t>Level of Authorization</t>
   </si>
   <si>
+    <t>Enablers</t>
+  </si>
+  <si>
+    <t>Enabler services provided</t>
+  </si>
+  <si>
+    <t>Application data</t>
+  </si>
+  <si>
     <t>Enablers2</t>
-  </si>
-  <si>
-    <t>Enabler services provided</t>
-  </si>
-  <si>
-    <t>Application data</t>
-  </si>
-  <si>
-    <t>Enablers</t>
-  </si>
-  <si>
-    <t>OpenApi</t>
   </si>
   <si>
     <t>OpenApi messages</t>
@@ -221,13 +234,15 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:D5" totalsRowShown="0">
-  <autoFilter ref="A1:D5"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:F5" totalsRowShown="0">
+  <autoFilter ref="A1:F5"/>
+  <tableColumns count="6">
     <tableColumn id="1" name="ID"/>
-    <tableColumn id="2" name="Description"/>
-    <tableColumn id="3" name="Trust Level"/>
-    <tableColumn id="4" name="Microservice"/>
+    <tableColumn id="2" name="Direction"/>
+    <tableColumn id="3" name="Description"/>
+    <tableColumn id="4" name="Asset Name"/>
+    <tableColumn id="5" name="Trust Level"/>
+    <tableColumn id="6" name="Microservice"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -268,6 +283,16 @@
     <tableColumn id="5" name="Vector"/>
     <tableColumn id="6" name="Status"/>
     <tableColumn id="7" name="Mitigations"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A1:A2" totalsRowShown="0">
+  <autoFilter ref="A1:A2"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -711,85 +736,114 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>18</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+      <c r="F1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
         <v>22</v>
       </c>
-      <c r="D2" t="s">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
+      <c r="C5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
       <c r="D5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+      <c r="F5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -823,38 +877,38 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -887,10 +941,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -923,22 +977,22 @@
         <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="F1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7">
@@ -946,22 +1000,22 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:7">
@@ -969,114 +1023,143 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>41</v>
-      </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" t="s">
         <v>46</v>
       </c>
-      <c r="C4" t="s">
-        <v>40</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
-        <v>42</v>
-      </c>
       <c r="F4" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E5" t="s">
         <v>46</v>
       </c>
-      <c r="C5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>42</v>
-      </c>
       <c r="F5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>44</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
         <v>46</v>
       </c>
-      <c r="C6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>42</v>
-      </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
         <v>46</v>
       </c>
-      <c r="C7" t="s">
-        <v>40</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>42</v>
-      </c>
       <c r="F7" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>44</v>
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix id error on diagram
</commit_message>
<xml_diff>
--- a/exemples/output/A1_Diagram1.xlsx
+++ b/exemples/output/A1_Diagram1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="54">
   <si>
     <t>Name</t>
   </si>
@@ -30,6 +30,9 @@
     <t>Trust Level</t>
   </si>
   <si>
+    <t>Out of scope</t>
+  </si>
+  <si>
     <t>MyProcess</t>
   </si>
   <si>
@@ -39,10 +42,16 @@
     <t>Operational</t>
   </si>
   <si>
+    <t>No</t>
+  </si>
+  <si>
     <t>RabbitMq</t>
   </si>
   <si>
     <t>Message broker</t>
+  </si>
+  <si>
+    <t>Yes</t>
   </si>
   <si>
     <t>Prometheus</t>
@@ -222,12 +231,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C12" totalsRowShown="0">
-  <autoFilter ref="A1:C12"/>
-  <tableColumns count="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D12" totalsRowShown="0">
+  <autoFilter ref="A1:D12"/>
+  <tableColumns count="4">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Description"/>
     <tableColumn id="3" name="Trust Level"/>
+    <tableColumn id="4" name="Out of scope"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium23" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -583,7 +593,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -592,9 +602,10 @@
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -604,126 +615,162 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
+      <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" t="s">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>9</v>
-      </c>
       <c r="C10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>6</v>
+      </c>
+      <c r="D11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="D12" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -752,99 +799,99 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
       </c>
       <c r="F1" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D4" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -871,44 +918,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -941,10 +988,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -974,163 +1021,163 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="F1" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="E2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="F2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E3" t="s">
-        <v>46</v>
-      </c>
       <c r="F3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
+        <v>49</v>
+      </c>
+      <c r="F4" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-      <c r="F4" t="s">
-        <v>47</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E5" t="s">
-        <v>46</v>
-      </c>
-      <c r="F5" t="s">
-        <v>47</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" t="s">
-        <v>47</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>49</v>
+      </c>
+      <c r="F7" t="s">
         <v>50</v>
       </c>
-      <c r="C7" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F7" t="s">
-        <v>47</v>
-      </c>
       <c r="G7" s="1" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
   </sheetData>
@@ -1159,7 +1206,7 @@
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>